<commit_message>
docs: requirement list 수정
</commit_message>
<xml_diff>
--- a/강지완/Requirement_list_final_강지완.xlsx
+++ b/강지완/Requirement_list_final_강지완.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lecture\24-1\소프트웨어공학\팀플\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\SE_Team2\강지완\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D516F52-D1F1-485F-9B72-B35EC46AEF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714B299E-654A-45AD-A921-244E7D1CEEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9A1A4C-40C9-46E0-9101-937DFF5848E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9A1A4C-40C9-46E0-9101-937DFF5848E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,10 +82,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>관리자는 자전거 대여소 리스트 조회 화면에서 원하는 대여소 항목을 선택하면 등록시 입력한 상세 내용을 볼 수 있다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>관리자는 등록된 자전거 대여소 리스트를 조회할 수 있다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -95,6 +91,10 @@
   </si>
   <si>
     <t>관리자는 대여소 리스트 조회 화면에서 특정 대여소 항목을 선택해서 삭제할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자는 원하는 대여소 항목을 선택하면 등록시 입력한 상세 내용을 볼 수 있다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -543,7 +543,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -601,10 +601,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -612,7 +612,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
@@ -623,7 +623,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>

</xml_diff>